<commit_message>
Update AffordabilityTables - TY25.xlsx
</commit_message>
<xml_diff>
--- a/AffordabilityTables - TY25.xlsx
+++ b/AffordabilityTables - TY25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Documents\GitHub\taxaide-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8813EE-2D1B-4FC0-94AE-3C1E2284DCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23866C5-5C86-4C8C-ABAA-D4B886E275D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9270" yWindow="405" windowWidth="18555" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9435" yWindow="1095" windowWidth="19365" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,6 +478,8 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -496,26 +498,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E63"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,10 +858,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="54">
+      <c r="A6" s="42">
         <v>22590</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="41">
         <v>0</v>
       </c>
       <c r="C6">
@@ -875,18 +875,18 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="54">
+      <c r="G6" s="42">
         <v>22590</v>
       </c>
-      <c r="H6" s="53">
+      <c r="H6" s="41">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="54">
+      <c r="A7" s="42">
         <v>30120</v>
       </c>
-      <c r="B7" s="53">
+      <c r="B7" s="41">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="C7">
@@ -897,21 +897,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">   {incomelimit:30120, percentage:0.029},</v>
       </c>
-      <c r="F7" s="54">
+      <c r="F7" s="42">
         <v>22591</v>
       </c>
-      <c r="G7" s="54">
+      <c r="G7" s="42">
         <v>30120</v>
       </c>
-      <c r="H7" s="53">
+      <c r="H7" s="41">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="54">
+      <c r="A8" s="42">
         <v>37650</v>
       </c>
-      <c r="B8" s="53">
+      <c r="B8" s="41">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C8">
@@ -922,21 +922,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">   {incomelimit:37650, percentage:0.042},</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="42">
         <v>30121</v>
       </c>
-      <c r="G8" s="54">
+      <c r="G8" s="42">
         <v>37650</v>
       </c>
-      <c r="H8" s="53">
+      <c r="H8" s="41">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="54">
+      <c r="A9" s="42">
         <v>45180</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="41">
         <v>0.05</v>
       </c>
       <c r="C9">
@@ -947,21 +947,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">   {incomelimit:45180, percentage:0.05},</v>
       </c>
-      <c r="F9" s="54">
+      <c r="F9" s="42">
         <v>37651</v>
       </c>
-      <c r="G9" s="54">
+      <c r="G9" s="42">
         <v>45180</v>
       </c>
-      <c r="H9" s="53">
+      <c r="H9" s="41">
         <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="54">
+      <c r="A10" s="42">
         <v>52710</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B10" s="41">
         <v>7.4499999999999997E-2</v>
       </c>
       <c r="C10">
@@ -972,21 +972,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">   {incomelimit:52710, percentage:0.0745},</v>
       </c>
-      <c r="F10" s="54">
+      <c r="F10" s="42">
         <v>45181</v>
       </c>
-      <c r="G10" s="54">
+      <c r="G10" s="42">
         <v>52710</v>
       </c>
-      <c r="H10" s="53">
+      <c r="H10" s="41">
         <v>7.4499999999999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="54">
+      <c r="A11" s="42">
         <v>60240</v>
       </c>
-      <c r="B11" s="53">
+      <c r="B11" s="41">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="C11">
@@ -997,21 +997,21 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">   {incomelimit:60240, percentage:0.076},</v>
       </c>
-      <c r="F11" s="54">
+      <c r="F11" s="42">
         <v>52711</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="42">
         <v>60240</v>
       </c>
-      <c r="H11" s="53">
+      <c r="H11" s="41">
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="54">
+      <c r="A12" s="42">
         <v>60241</v>
       </c>
-      <c r="B12" s="53">
+      <c r="B12" s="41">
         <v>0.08</v>
       </c>
       <c r="C12">
@@ -1022,13 +1022,13 @@
         <f>CONCATENATE("   {incomelimit:",A12,", percentage:",C12,"}")</f>
         <v xml:space="preserve">   {incomelimit:60241, percentage:0.08}</v>
       </c>
-      <c r="F12" s="54">
+      <c r="F12" s="42">
         <v>60241</v>
       </c>
-      <c r="G12" s="54">
+      <c r="G12" s="42">
         <v>60241</v>
       </c>
-      <c r="H12" s="53">
+      <c r="H12" s="41">
         <v>0.08</v>
       </c>
     </row>
@@ -1045,10 +1045,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="54">
+      <c r="A15" s="42">
         <v>30660</v>
       </c>
-      <c r="B15" s="53">
+      <c r="B15" s="41">
         <v>0</v>
       </c>
       <c r="C15">
@@ -1059,21 +1059,21 @@
         <f t="shared" ref="E15:E20" si="3">CONCATENATE("   {incomelimit:",A15,", percentage:",C15,"},")</f>
         <v xml:space="preserve">   {incomelimit:30660, percentage:0},</v>
       </c>
-      <c r="F15" s="54">
+      <c r="F15" s="42">
         <v>0</v>
       </c>
-      <c r="G15" s="54">
+      <c r="G15" s="42">
         <v>30660</v>
       </c>
-      <c r="H15" s="53">
+      <c r="H15" s="41">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="54">
+      <c r="A16" s="42">
         <v>40880</v>
       </c>
-      <c r="B16" s="53">
+      <c r="B16" s="41">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="C16">
@@ -1084,21 +1084,21 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">   {incomelimit:40880, percentage:0.043},</v>
       </c>
-      <c r="F16" s="54">
+      <c r="F16" s="42">
         <v>30661</v>
       </c>
-      <c r="G16" s="54">
+      <c r="G16" s="42">
         <v>40880</v>
       </c>
-      <c r="H16" s="53">
+      <c r="H16" s="41">
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="54">
+      <c r="A17" s="42">
         <v>51100</v>
       </c>
-      <c r="B17" s="53">
+      <c r="B17" s="41">
         <v>6.2E-2</v>
       </c>
       <c r="C17">
@@ -1109,21 +1109,21 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">   {incomelimit:51100, percentage:0.062},</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="42">
         <v>40881</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="42">
         <v>51100</v>
       </c>
-      <c r="H17" s="53">
+      <c r="H17" s="41">
         <v>6.2E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="54">
+      <c r="A18" s="42">
         <v>61320</v>
       </c>
-      <c r="B18" s="53">
+      <c r="B18" s="41">
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="C18">
@@ -1134,21 +1134,21 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">   {incomelimit:61320, percentage:0.074},</v>
       </c>
-      <c r="F18" s="54">
+      <c r="F18" s="42">
         <v>51101</v>
       </c>
-      <c r="G18" s="54">
+      <c r="G18" s="42">
         <v>61320</v>
       </c>
-      <c r="H18" s="53">
+      <c r="H18" s="41">
         <v>7.3999999999999996E-2</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="54">
+      <c r="A19" s="42">
         <v>71540</v>
       </c>
-      <c r="B19" s="53">
+      <c r="B19" s="41">
         <v>7.4499999999999997E-2</v>
       </c>
       <c r="C19">
@@ -1159,21 +1159,21 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">   {incomelimit:71540, percentage:0.0745},</v>
       </c>
-      <c r="F19" s="54">
+      <c r="F19" s="42">
         <v>61321</v>
       </c>
-      <c r="G19" s="54">
+      <c r="G19" s="42">
         <v>71540</v>
       </c>
-      <c r="H19" s="53">
+      <c r="H19" s="41">
         <v>7.4499999999999997E-2</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="54">
+      <c r="A20" s="42">
         <v>81760</v>
       </c>
-      <c r="B20" s="53">
+      <c r="B20" s="41">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="C20">
@@ -1184,21 +1184,21 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">   {incomelimit:81760, percentage:0.076},</v>
       </c>
-      <c r="F20" s="54">
+      <c r="F20" s="42">
         <v>71541</v>
       </c>
-      <c r="G20" s="54">
+      <c r="G20" s="42">
         <v>81760</v>
       </c>
-      <c r="H20" s="53">
+      <c r="H20" s="41">
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="54">
+      <c r="A21" s="42">
         <v>81761</v>
       </c>
-      <c r="B21" s="53">
+      <c r="B21" s="41">
         <v>0.08</v>
       </c>
       <c r="C21">
@@ -1209,13 +1209,13 @@
         <f>CONCATENATE("   {incomelimit:",A21,", percentage:",C21,"}")</f>
         <v xml:space="preserve">   {incomelimit:81761, percentage:0.08}</v>
       </c>
-      <c r="F21" s="54">
+      <c r="F21" s="42">
         <v>81761</v>
       </c>
-      <c r="G21" s="54">
+      <c r="G21" s="42">
         <v>81761</v>
       </c>
-      <c r="H21" s="53">
+      <c r="H21" s="41">
         <v>0.08</v>
       </c>
     </row>
@@ -1227,24 +1227,24 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E23" t="str">
-        <f>CONCATENATE("_AffordTab3Plus[_TY] = [")</f>
-        <v>_AffordTab3Plus[_TY] = [</v>
-      </c>
-      <c r="F23" s="54">
+        <f>CONCATENATE("_AffordTab3[_TY] = [")</f>
+        <v>_AffordTab3[_TY] = [</v>
+      </c>
+      <c r="F23" s="42">
         <v>0</v>
       </c>
-      <c r="G23" s="54">
+      <c r="G23" s="42">
         <v>38730</v>
       </c>
-      <c r="H23" s="53">
+      <c r="H23" s="41">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="54">
+      <c r="A24" s="42">
         <v>38730</v>
       </c>
-      <c r="B24" s="53">
+      <c r="B24" s="41">
         <v>0</v>
       </c>
       <c r="C24">
@@ -1255,21 +1255,21 @@
         <f t="shared" ref="E24:E29" si="5">CONCATENATE("   {incomelimit:",A24,", percentage:",C24,"},")</f>
         <v xml:space="preserve">   {incomelimit:38730, percentage:0},</v>
       </c>
-      <c r="F24" s="54">
+      <c r="F24" s="42">
         <v>38731</v>
       </c>
-      <c r="G24" s="54">
+      <c r="G24" s="42">
         <v>51640</v>
       </c>
-      <c r="H24" s="53">
+      <c r="H24" s="41">
         <v>3.4500000000000003E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="54">
+      <c r="A25" s="42">
         <v>51640</v>
       </c>
-      <c r="B25" s="53">
+      <c r="B25" s="41">
         <v>3.4500000000000003E-2</v>
       </c>
       <c r="C25">
@@ -1280,21 +1280,21 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">   {incomelimit:51640, percentage:0.0345},</v>
       </c>
-      <c r="F25" s="54">
+      <c r="F25" s="42">
         <v>51641</v>
       </c>
-      <c r="G25" s="54">
+      <c r="G25" s="42">
         <v>64550</v>
       </c>
-      <c r="H25" s="53">
+      <c r="H25" s="41">
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="54">
+      <c r="A26" s="42">
         <v>64550</v>
       </c>
-      <c r="B26" s="53">
+      <c r="B26" s="41">
         <v>4.9500000000000002E-2</v>
       </c>
       <c r="C26">
@@ -1305,21 +1305,21 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">   {incomelimit:64550, percentage:0.0495},</v>
       </c>
-      <c r="F26" s="54">
+      <c r="F26" s="42">
         <v>64551</v>
       </c>
-      <c r="G26" s="54">
+      <c r="G26" s="42">
         <v>77460</v>
       </c>
-      <c r="H26" s="53">
+      <c r="H26" s="41">
         <v>5.8500000000000003E-2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="54">
+      <c r="A27" s="42">
         <v>77460</v>
       </c>
-      <c r="B27" s="53">
+      <c r="B27" s="41">
         <v>5.8500000000000003E-2</v>
       </c>
       <c r="C27">
@@ -1330,21 +1330,21 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">   {incomelimit:77460, percentage:0.0585},</v>
       </c>
-      <c r="F27" s="54">
+      <c r="F27" s="42">
         <v>77461</v>
       </c>
-      <c r="G27" s="54">
+      <c r="G27" s="42">
         <v>90370</v>
       </c>
-      <c r="H27" s="53">
+      <c r="H27" s="41">
         <v>7.4499999999999997E-2</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="54">
+      <c r="A28" s="42">
         <v>90370</v>
       </c>
-      <c r="B28" s="53">
+      <c r="B28" s="41">
         <v>7.4499999999999997E-2</v>
       </c>
       <c r="C28">
@@ -1355,21 +1355,21 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">   {incomelimit:90370, percentage:0.0745},</v>
       </c>
-      <c r="F28" s="54">
+      <c r="F28" s="42">
         <v>90371</v>
       </c>
-      <c r="G28" s="54">
+      <c r="G28" s="42">
         <v>103280</v>
       </c>
-      <c r="H28" s="53">
+      <c r="H28" s="41">
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="54">
+      <c r="A29" s="42">
         <v>103280</v>
       </c>
-      <c r="B29" s="53">
+      <c r="B29" s="41">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="C29">
@@ -1380,21 +1380,21 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve">   {incomelimit:103280, percentage:0.076},</v>
       </c>
-      <c r="F29" s="54">
+      <c r="F29" s="42">
         <v>103281</v>
       </c>
-      <c r="G29" s="54">
+      <c r="G29" s="42">
         <v>103281</v>
       </c>
-      <c r="H29" s="53">
+      <c r="H29" s="41">
         <v>0.08</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="54">
+      <c r="A30" s="42">
         <v>103281</v>
       </c>
-      <c r="B30" s="53">
+      <c r="B30" s="41">
         <v>0.08</v>
       </c>
       <c r="C30">
@@ -1422,24 +1422,24 @@
       <c r="F33" t="s">
         <v>31</v>
       </c>
-      <c r="G33" s="54">
+      <c r="G33" s="42">
         <v>350</v>
       </c>
-      <c r="H33" s="54">
+      <c r="H33" s="42">
         <v>699</v>
       </c>
-      <c r="I33" s="54">
+      <c r="I33" s="42">
         <v>905</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="54">
+      <c r="A34" s="42">
         <v>350</v>
       </c>
-      <c r="B34" s="54">
+      <c r="B34" s="42">
         <v>699</v>
       </c>
-      <c r="C34" s="54">
+      <c r="C34" s="42">
         <v>905</v>
       </c>
       <c r="D34" s="6"/>
@@ -1450,24 +1450,24 @@
       <c r="F34" t="s">
         <v>32</v>
       </c>
-      <c r="G34" s="54">
+      <c r="G34" s="42">
         <v>374</v>
       </c>
-      <c r="H34" s="54">
+      <c r="H34" s="42">
         <v>748</v>
       </c>
-      <c r="I34" s="54">
+      <c r="I34" s="42">
         <v>956</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="54">
+      <c r="A35" s="42">
         <v>374</v>
       </c>
-      <c r="B35" s="54">
+      <c r="B35" s="42">
         <v>748</v>
       </c>
-      <c r="C35" s="54">
+      <c r="C35" s="42">
         <v>956</v>
       </c>
       <c r="D35" s="6"/>
@@ -1478,24 +1478,24 @@
       <c r="F35" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="54">
+      <c r="G35" s="42">
         <v>384</v>
       </c>
-      <c r="H35" s="54">
+      <c r="H35" s="42">
         <v>767</v>
       </c>
-      <c r="I35" s="54">
+      <c r="I35" s="42">
         <v>976</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="54">
+      <c r="A36" s="42">
         <v>384</v>
       </c>
-      <c r="B36" s="54">
+      <c r="B36" s="42">
         <v>767</v>
       </c>
-      <c r="C36" s="54">
+      <c r="C36" s="42">
         <v>976</v>
       </c>
       <c r="D36" s="6"/>
@@ -1506,24 +1506,24 @@
       <c r="F36" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="54">
+      <c r="G36" s="42">
         <v>411</v>
       </c>
-      <c r="H36" s="54">
+      <c r="H36" s="42">
         <v>821</v>
       </c>
-      <c r="I36" s="54">
+      <c r="I36" s="42">
         <v>1029</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="54">
+      <c r="A37" s="42">
         <v>411</v>
       </c>
-      <c r="B37" s="54">
+      <c r="B37" s="42">
         <v>821</v>
       </c>
-      <c r="C37" s="54">
+      <c r="C37" s="42">
         <v>1029</v>
       </c>
       <c r="D37" s="6"/>
@@ -1534,24 +1534,24 @@
       <c r="F37" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="54">
+      <c r="G37" s="42">
         <v>469</v>
       </c>
-      <c r="H37" s="54">
+      <c r="H37" s="42">
         <v>938</v>
       </c>
-      <c r="I37" s="54">
+      <c r="I37" s="42">
         <v>1146</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="54">
+      <c r="A38" s="42">
         <v>469</v>
       </c>
-      <c r="B38" s="54">
+      <c r="B38" s="42">
         <v>938</v>
       </c>
-      <c r="C38" s="54">
+      <c r="C38" s="42">
         <v>1146</v>
       </c>
       <c r="D38" s="6"/>
@@ -1562,24 +1562,24 @@
       <c r="F38" t="s">
         <v>36</v>
       </c>
-      <c r="G38" s="54">
+      <c r="G38" s="42">
         <v>545</v>
       </c>
-      <c r="H38" s="54">
+      <c r="H38" s="42">
         <v>1089</v>
       </c>
-      <c r="I38" s="54">
+      <c r="I38" s="42">
         <v>1298</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="54">
+      <c r="A39" s="42">
         <v>545</v>
       </c>
-      <c r="B39" s="54">
+      <c r="B39" s="42">
         <v>1089</v>
       </c>
-      <c r="C39" s="54">
+      <c r="C39" s="42">
         <v>1298</v>
       </c>
       <c r="D39" s="6"/>
@@ -1590,24 +1590,24 @@
       <c r="F39" t="s">
         <v>26</v>
       </c>
-      <c r="G39" s="54">
+      <c r="G39" s="42">
         <v>561</v>
       </c>
-      <c r="H39" s="54">
+      <c r="H39" s="42">
         <v>1121</v>
       </c>
-      <c r="I39" s="54">
+      <c r="I39" s="42">
         <v>1330</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="54">
+      <c r="A40" s="42">
         <v>561</v>
       </c>
-      <c r="B40" s="54">
+      <c r="B40" s="42">
         <v>1121</v>
       </c>
-      <c r="C40" s="54">
+      <c r="C40" s="42">
         <v>1330</v>
       </c>
       <c r="D40" s="6"/>
@@ -1632,24 +1632,24 @@
       <c r="F44" t="s">
         <v>31</v>
       </c>
-      <c r="G44" s="54">
+      <c r="G44" s="42">
         <v>320</v>
       </c>
-      <c r="H44" s="54">
+      <c r="H44" s="42">
         <v>639</v>
       </c>
-      <c r="I44" s="54">
+      <c r="I44" s="42">
         <v>825</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="54">
+      <c r="A45" s="42">
         <v>320</v>
       </c>
-      <c r="B45" s="54">
+      <c r="B45" s="42">
         <v>639</v>
       </c>
-      <c r="C45" s="54">
+      <c r="C45" s="42">
         <v>825</v>
       </c>
       <c r="D45" s="40"/>
@@ -1660,24 +1660,24 @@
       <c r="F45" t="s">
         <v>32</v>
       </c>
-      <c r="G45" s="54">
+      <c r="G45" s="42">
         <v>334</v>
       </c>
-      <c r="H45" s="54">
+      <c r="H45" s="42">
         <v>668</v>
       </c>
-      <c r="I45" s="54">
+      <c r="I45" s="42">
         <v>854</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="54">
+      <c r="A46" s="42">
         <v>334</v>
       </c>
-      <c r="B46" s="54">
+      <c r="B46" s="42">
         <v>668</v>
       </c>
-      <c r="C46" s="54">
+      <c r="C46" s="42">
         <v>854</v>
       </c>
       <c r="D46" s="40"/>
@@ -1688,24 +1688,24 @@
       <c r="F46" t="s">
         <v>33</v>
       </c>
-      <c r="G46" s="54">
+      <c r="G46" s="42">
         <v>343</v>
       </c>
-      <c r="H46" s="54">
+      <c r="H46" s="42">
         <v>685</v>
       </c>
-      <c r="I46" s="54">
+      <c r="I46" s="42">
         <v>871</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="54">
+      <c r="A47" s="42">
         <v>343</v>
       </c>
-      <c r="B47" s="54">
+      <c r="B47" s="42">
         <v>685</v>
       </c>
-      <c r="C47" s="54">
+      <c r="C47" s="42">
         <v>871</v>
       </c>
       <c r="D47" s="40"/>
@@ -1716,24 +1716,24 @@
       <c r="F47" t="s">
         <v>34</v>
       </c>
-      <c r="G47" s="54">
+      <c r="G47" s="42">
         <v>367</v>
       </c>
-      <c r="H47" s="54">
+      <c r="H47" s="42">
         <v>733</v>
       </c>
-      <c r="I47" s="54">
+      <c r="I47" s="42">
         <v>920</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="54">
+      <c r="A48" s="42">
         <v>367</v>
       </c>
-      <c r="B48" s="54">
+      <c r="B48" s="42">
         <v>733</v>
       </c>
-      <c r="C48" s="54">
+      <c r="C48" s="42">
         <v>920</v>
       </c>
       <c r="D48" s="40"/>
@@ -1744,24 +1744,24 @@
       <c r="F48" t="s">
         <v>35</v>
       </c>
-      <c r="G48" s="54">
+      <c r="G48" s="42">
         <v>419</v>
       </c>
-      <c r="H48" s="54">
+      <c r="H48" s="42">
         <v>838</v>
       </c>
-      <c r="I48" s="54">
+      <c r="I48" s="42">
         <v>1024</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="54">
+      <c r="A49" s="42">
         <v>419</v>
       </c>
-      <c r="B49" s="54">
+      <c r="B49" s="42">
         <v>838</v>
       </c>
-      <c r="C49" s="54">
+      <c r="C49" s="42">
         <v>1024</v>
       </c>
       <c r="D49" s="40"/>
@@ -1772,24 +1772,24 @@
       <c r="F49" t="s">
         <v>36</v>
       </c>
-      <c r="G49" s="54">
+      <c r="G49" s="42">
         <v>487</v>
       </c>
-      <c r="H49" s="54">
+      <c r="H49" s="42">
         <v>973</v>
       </c>
-      <c r="I49" s="54">
+      <c r="I49" s="42">
         <v>1159</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="54">
+      <c r="A50" s="42">
         <v>487</v>
       </c>
-      <c r="B50" s="54">
+      <c r="B50" s="42">
         <v>973</v>
       </c>
-      <c r="C50" s="54">
+      <c r="C50" s="42">
         <v>1159</v>
       </c>
       <c r="D50" s="40"/>
@@ -1800,24 +1800,24 @@
       <c r="F50" t="s">
         <v>26</v>
       </c>
-      <c r="G50" s="54">
+      <c r="G50" s="42">
         <v>501</v>
       </c>
-      <c r="H50" s="54">
+      <c r="H50" s="42">
         <v>1002</v>
       </c>
-      <c r="I50" s="54">
+      <c r="I50" s="42">
         <v>1188</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="54">
+      <c r="A51" s="42">
         <v>501</v>
       </c>
-      <c r="B51" s="54">
+      <c r="B51" s="42">
         <v>1002</v>
       </c>
-      <c r="C51" s="54">
+      <c r="C51" s="42">
         <v>1188</v>
       </c>
       <c r="D51" s="40"/>
@@ -1839,13 +1839,13 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="54">
+      <c r="A56" s="42">
         <v>445</v>
       </c>
-      <c r="B56" s="54">
+      <c r="B56" s="42">
         <v>890</v>
       </c>
-      <c r="C56" s="54">
+      <c r="C56" s="42">
         <v>1151</v>
       </c>
       <c r="D56" s="40"/>
@@ -1856,24 +1856,24 @@
       <c r="F56" t="s">
         <v>31</v>
       </c>
-      <c r="G56" s="54">
+      <c r="G56" s="42">
         <v>445</v>
       </c>
-      <c r="H56" s="54">
+      <c r="H56" s="42">
         <v>890</v>
       </c>
-      <c r="I56" s="54">
+      <c r="I56" s="42">
         <v>1151</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="54">
+      <c r="A57" s="42">
         <v>539</v>
       </c>
-      <c r="B57" s="54">
+      <c r="B57" s="42">
         <v>1078</v>
       </c>
-      <c r="C57" s="54">
+      <c r="C57" s="42">
         <v>1378</v>
       </c>
       <c r="D57" s="40"/>
@@ -1884,24 +1884,24 @@
       <c r="F57" t="s">
         <v>32</v>
       </c>
-      <c r="G57" s="54">
+      <c r="G57" s="42">
         <v>539</v>
       </c>
-      <c r="H57" s="54">
+      <c r="H57" s="42">
         <v>1078</v>
       </c>
-      <c r="I57" s="54">
+      <c r="I57" s="42">
         <v>1378</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="54">
+      <c r="A58" s="42">
         <v>553</v>
       </c>
-      <c r="B58" s="54">
+      <c r="B58" s="42">
         <v>1106</v>
       </c>
-      <c r="C58" s="54">
+      <c r="C58" s="42">
         <v>1406</v>
       </c>
       <c r="D58" s="40"/>
@@ -1912,24 +1912,24 @@
       <c r="F58" t="s">
         <v>33</v>
       </c>
-      <c r="G58" s="54">
+      <c r="G58" s="42">
         <v>553</v>
       </c>
-      <c r="H58" s="54">
+      <c r="H58" s="42">
         <v>1106</v>
       </c>
-      <c r="I58" s="54">
+      <c r="I58" s="42">
         <v>1406</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="54">
+      <c r="A59" s="42">
         <v>592</v>
       </c>
-      <c r="B59" s="54">
+      <c r="B59" s="42">
         <v>1183</v>
       </c>
-      <c r="C59" s="54">
+      <c r="C59" s="42">
         <v>1484</v>
       </c>
       <c r="D59" s="40"/>
@@ -1940,24 +1940,24 @@
       <c r="F59" t="s">
         <v>34</v>
       </c>
-      <c r="G59" s="54">
+      <c r="G59" s="42">
         <v>592</v>
       </c>
-      <c r="H59" s="54">
+      <c r="H59" s="42">
         <v>1183</v>
       </c>
-      <c r="I59" s="54">
+      <c r="I59" s="42">
         <v>1484</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="54">
+      <c r="A60" s="42">
         <v>676</v>
       </c>
-      <c r="B60" s="54">
+      <c r="B60" s="42">
         <v>1351</v>
       </c>
-      <c r="C60" s="54">
+      <c r="C60" s="42">
         <v>1652</v>
       </c>
       <c r="D60" s="40"/>
@@ -1968,24 +1968,24 @@
       <c r="F60" t="s">
         <v>35</v>
       </c>
-      <c r="G60" s="54">
+      <c r="G60" s="42">
         <v>676</v>
       </c>
-      <c r="H60" s="54">
+      <c r="H60" s="42">
         <v>1351</v>
       </c>
-      <c r="I60" s="54">
+      <c r="I60" s="42">
         <v>1652</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="54">
+      <c r="A61" s="42">
         <v>785</v>
       </c>
-      <c r="B61" s="54">
+      <c r="B61" s="42">
         <v>1570</v>
       </c>
-      <c r="C61" s="54">
+      <c r="C61" s="42">
         <v>1870</v>
       </c>
       <c r="D61" s="40"/>
@@ -1996,24 +1996,24 @@
       <c r="F61" t="s">
         <v>36</v>
       </c>
-      <c r="G61" s="54">
+      <c r="G61" s="42">
         <v>785</v>
       </c>
-      <c r="H61" s="54">
+      <c r="H61" s="42">
         <v>1570</v>
       </c>
-      <c r="I61" s="54">
+      <c r="I61" s="42">
         <v>1870</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="54">
+      <c r="A62" s="42">
         <v>808</v>
       </c>
-      <c r="B62" s="54">
+      <c r="B62" s="42">
         <v>1616</v>
       </c>
-      <c r="C62" s="54">
+      <c r="C62" s="42">
         <v>1917</v>
       </c>
       <c r="D62" s="40"/>
@@ -2024,13 +2024,13 @@
       <c r="F62" t="s">
         <v>26</v>
       </c>
-      <c r="G62" s="54">
+      <c r="G62" s="42">
         <v>808</v>
       </c>
-      <c r="H62" s="54">
+      <c r="H62" s="42">
         <v>1616</v>
       </c>
-      <c r="I62" s="54">
+      <c r="I62" s="42">
         <v>1917</v>
       </c>
     </row>
@@ -2057,13 +2057,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3"/>
@@ -2078,9 +2078,9 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="46"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -2344,13 +2344,13 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="3"/>
@@ -2363,9 +2363,9 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="46"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="4" t="s">
         <v>3</v>
       </c>
@@ -2619,20 +2619,20 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="3"/>
-      <c r="E31" s="47" t="s">
+      <c r="E31" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="47" t="s">
+      <c r="F31" s="53" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="35" t="s">
@@ -2649,14 +2649,14 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="46"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="48"/>
       <c r="D32" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
       <c r="H32" s="14" t="s">
         <v>20</v>
       </c>
@@ -2881,21 +2881,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>